<commit_message>
Caricamento Classifiche sere A e B, implementazione confronto dati Bench per serie B e calibrazione config tier
</commit_message>
<xml_diff>
--- a/docs/import csv.xlsx
+++ b/docs/import csv.xlsx
@@ -5,20 +5,25 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\fantaproject\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FD17A7-CEFF-42A2-93F5-7977A684EBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D318D763-C952-4F8D-95EE-8A9E7C8F829D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{E663C83A-6280-478F-BE17-E18937A9D031}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="652" firstSheet="2" activeTab="10" xr2:uid="{E663C83A-6280-478F-BE17-E18937A9D031}"/>
   </bookViews>
   <sheets>
     <sheet name="tracciato" sheetId="1" r:id="rId1"/>
     <sheet name="2020-21 A" sheetId="4" r:id="rId2"/>
     <sheet name="21-22 A" sheetId="2" r:id="rId3"/>
     <sheet name="22-23 A" sheetId="3" r:id="rId4"/>
-    <sheet name="2022-23 B" sheetId="5" r:id="rId5"/>
-    <sheet name="2023-24 B" sheetId="6" r:id="rId6"/>
+    <sheet name="2020-21 B" sheetId="7" r:id="rId5"/>
+    <sheet name="2021-22 B" sheetId="8" r:id="rId6"/>
+    <sheet name="2022-23 B" sheetId="5" r:id="rId7"/>
+    <sheet name="2023-24 B" sheetId="6" r:id="rId8"/>
+    <sheet name="2024-25 B" sheetId="9" r:id="rId9"/>
+    <sheet name="2024-25 A" sheetId="11" r:id="rId10"/>
+    <sheet name="2023-24 A" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="92">
   <si>
     <t>NomeSquadraDB</t>
   </si>
@@ -269,6 +274,54 @@
   </si>
   <si>
     <t>Lecco</t>
+  </si>
+  <si>
+    <t>Squadra</t>
+  </si>
+  <si>
+    <t>Pt</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Chievo</t>
+  </si>
+  <si>
+    <t>L.R. Vicenza</t>
+  </si>
+  <si>
+    <t>Pordenone</t>
+  </si>
+  <si>
+    <t>Pescara</t>
+  </si>
+  <si>
+    <t>Virtus Entella</t>
+  </si>
+  <si>
+    <t>Alessandria</t>
+  </si>
+  <si>
+    <t>L.R.Vicenza</t>
+  </si>
+  <si>
+    <t>Pos</t>
+  </si>
+  <si>
+    <t>JuveStabia</t>
+  </si>
+  <si>
+    <t>Cesena</t>
+  </si>
+  <si>
+    <t>Carrarese</t>
+  </si>
+  <si>
+    <t>Mantova</t>
+  </si>
+  <si>
+    <t>Sudtirol</t>
   </si>
 </sst>
 </file>
@@ -798,6 +851,1254 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D092F27C-D20A-493B-8DCB-FB779B7904C2}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>82</v>
+      </c>
+      <c r="D2">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>27</v>
+      </c>
+      <c r="F2">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>81</v>
+      </c>
+      <c r="D3">
+        <v>79</v>
+      </c>
+      <c r="E3">
+        <v>35</v>
+      </c>
+      <c r="F3">
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>74</v>
+      </c>
+      <c r="D4">
+        <v>78</v>
+      </c>
+      <c r="E4">
+        <v>37</v>
+      </c>
+      <c r="F4">
+        <v>22</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>58</v>
+      </c>
+      <c r="E5">
+        <v>35</v>
+      </c>
+      <c r="F5">
+        <v>18</v>
+      </c>
+      <c r="G5">
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>69</v>
+      </c>
+      <c r="D6">
+        <v>56</v>
+      </c>
+      <c r="E6">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7">
+        <v>41</v>
+      </c>
+      <c r="F7">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>65</v>
+      </c>
+      <c r="D8">
+        <v>61</v>
+      </c>
+      <c r="E8">
+        <v>49</v>
+      </c>
+      <c r="F8">
+        <v>18</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>63</v>
+      </c>
+      <c r="D9">
+        <v>61</v>
+      </c>
+      <c r="E9">
+        <v>43</v>
+      </c>
+      <c r="F9">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>11</v>
+      </c>
+      <c r="I9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>57</v>
+      </c>
+      <c r="E10">
+        <v>47</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <v>49</v>
+      </c>
+      <c r="E11">
+        <v>52</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>15</v>
+      </c>
+      <c r="I11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>44</v>
+      </c>
+      <c r="D12">
+        <v>39</v>
+      </c>
+      <c r="E12">
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <v>14</v>
+      </c>
+      <c r="I12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>44</v>
+      </c>
+      <c r="D13">
+        <v>41</v>
+      </c>
+      <c r="E13">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+      <c r="H13">
+        <v>18</v>
+      </c>
+      <c r="I13">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>43</v>
+      </c>
+      <c r="D14">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <v>49</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>15</v>
+      </c>
+      <c r="I14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>37</v>
+      </c>
+      <c r="D15">
+        <v>34</v>
+      </c>
+      <c r="E15">
+        <v>66</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>21</v>
+      </c>
+      <c r="I15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>36</v>
+      </c>
+      <c r="D16">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <v>56</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+      <c r="I16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>44</v>
+      </c>
+      <c r="E17">
+        <v>58</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>27</v>
+      </c>
+      <c r="E18">
+        <v>58</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>20</v>
+      </c>
+      <c r="I18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <v>33</v>
+      </c>
+      <c r="E19">
+        <v>59</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>13</v>
+      </c>
+      <c r="H19">
+        <v>19</v>
+      </c>
+      <c r="I19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>29</v>
+      </c>
+      <c r="D20">
+        <v>32</v>
+      </c>
+      <c r="E20">
+        <v>56</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>14</v>
+      </c>
+      <c r="H20">
+        <v>19</v>
+      </c>
+      <c r="I20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>28</v>
+      </c>
+      <c r="E21">
+        <v>69</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <v>26</v>
+      </c>
+      <c r="I21">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3B8A6F-5270-4341-8524-AB2AA9D4F014}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>94</v>
+      </c>
+      <c r="D2">
+        <v>89</v>
+      </c>
+      <c r="E2">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>76</v>
+      </c>
+      <c r="E3">
+        <v>49</v>
+      </c>
+      <c r="F3">
+        <v>22</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>71</v>
+      </c>
+      <c r="D4">
+        <v>54</v>
+      </c>
+      <c r="E4">
+        <v>31</v>
+      </c>
+      <c r="F4">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>69</v>
+      </c>
+      <c r="D5">
+        <v>72</v>
+      </c>
+      <c r="E5">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>68</v>
+      </c>
+      <c r="D6">
+        <v>54</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>63</v>
+      </c>
+      <c r="D7">
+        <v>65</v>
+      </c>
+      <c r="E7">
+        <v>46</v>
+      </c>
+      <c r="F7">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>61</v>
+      </c>
+      <c r="D8">
+        <v>49</v>
+      </c>
+      <c r="E8">
+        <v>39</v>
+      </c>
+      <c r="F8">
+        <v>18</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>13</v>
+      </c>
+      <c r="I8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>61</v>
+      </c>
+      <c r="E9">
+        <v>46</v>
+      </c>
+      <c r="F9">
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>53</v>
+      </c>
+      <c r="D10">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <v>36</v>
+      </c>
+      <c r="F10">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>11</v>
+      </c>
+      <c r="I10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>53</v>
+      </c>
+      <c r="D11">
+        <v>55</v>
+      </c>
+      <c r="E11">
+        <v>48</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>11</v>
+      </c>
+      <c r="I11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>49</v>
+      </c>
+      <c r="D12">
+        <v>45</v>
+      </c>
+      <c r="E12">
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>13</v>
+      </c>
+      <c r="H12">
+        <v>13</v>
+      </c>
+      <c r="I12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <v>39</v>
+      </c>
+      <c r="E13">
+        <v>51</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>15</v>
+      </c>
+      <c r="I13">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>38</v>
+      </c>
+      <c r="E14">
+        <v>51</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <v>18</v>
+      </c>
+      <c r="I14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>32</v>
+      </c>
+      <c r="E15">
+        <v>54</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>16</v>
+      </c>
+      <c r="I15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>37</v>
+      </c>
+      <c r="D16">
+        <v>37</v>
+      </c>
+      <c r="E16">
+        <v>53</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>42</v>
+      </c>
+      <c r="E17">
+        <v>68</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>18</v>
+      </c>
+      <c r="I17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>36</v>
+      </c>
+      <c r="D18">
+        <v>29</v>
+      </c>
+      <c r="E18">
+        <v>54</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>20</v>
+      </c>
+      <c r="I18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>35</v>
+      </c>
+      <c r="D19">
+        <v>44</v>
+      </c>
+      <c r="E19">
+        <v>69</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>11</v>
+      </c>
+      <c r="H19">
+        <v>19</v>
+      </c>
+      <c r="I19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <v>43</v>
+      </c>
+      <c r="E20">
+        <v>75</v>
+      </c>
+      <c r="F20">
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <v>22</v>
+      </c>
+      <c r="I20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>32</v>
+      </c>
+      <c r="E21">
+        <v>81</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>11</v>
+      </c>
+      <c r="H21">
+        <v>25</v>
+      </c>
+      <c r="I21">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219E3C4F-5E5B-438F-B2AE-C9D0C9180D03}">
   <dimension ref="A1:I21"/>
@@ -2671,6 +3972,1260 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECFB767-8A85-4235-8EDB-CF7258422533}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>73</v>
+      </c>
+      <c r="D2">
+        <v>68</v>
+      </c>
+      <c r="E2">
+        <v>35</v>
+      </c>
+      <c r="F2">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>69</v>
+      </c>
+      <c r="D3">
+        <v>46</v>
+      </c>
+      <c r="E3">
+        <v>34</v>
+      </c>
+      <c r="F3">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>64</v>
+      </c>
+      <c r="D4">
+        <v>51</v>
+      </c>
+      <c r="E4">
+        <v>33</v>
+      </c>
+      <c r="F4">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>62</v>
+      </c>
+      <c r="D5">
+        <v>68</v>
+      </c>
+      <c r="E5">
+        <v>47</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>59</v>
+      </c>
+      <c r="D6">
+        <v>53</v>
+      </c>
+      <c r="E6">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>57</v>
+      </c>
+      <c r="D7">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>56</v>
+      </c>
+      <c r="D8">
+        <v>61</v>
+      </c>
+      <c r="E8">
+        <v>53</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>56</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="E9">
+        <v>37</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <v>42</v>
+      </c>
+      <c r="F10">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11">
+        <v>38</v>
+      </c>
+      <c r="E11">
+        <v>42</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>42</v>
+      </c>
+      <c r="E12">
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>48</v>
+      </c>
+      <c r="D13">
+        <v>48</v>
+      </c>
+      <c r="E13">
+        <v>53</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>48</v>
+      </c>
+      <c r="D14">
+        <v>46</v>
+      </c>
+      <c r="E14">
+        <v>44</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <v>14</v>
+      </c>
+      <c r="I14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>48</v>
+      </c>
+      <c r="D15">
+        <v>54</v>
+      </c>
+      <c r="E15">
+        <v>59</v>
+      </c>
+      <c r="F15">
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>45</v>
+      </c>
+      <c r="D16">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <v>39</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>48</v>
+      </c>
+      <c r="F17">
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <v>11</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>35</v>
+      </c>
+      <c r="D18">
+        <v>29</v>
+      </c>
+      <c r="E18">
+        <v>47</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>15</v>
+      </c>
+      <c r="I18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>31</v>
+      </c>
+      <c r="E19">
+        <v>57</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>22</v>
+      </c>
+      <c r="I19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>32</v>
+      </c>
+      <c r="D20">
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <v>60</v>
+      </c>
+      <c r="F20">
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>11</v>
+      </c>
+      <c r="H20">
+        <v>20</v>
+      </c>
+      <c r="I20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>23</v>
+      </c>
+      <c r="D21">
+        <v>30</v>
+      </c>
+      <c r="E21">
+        <v>64</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>11</v>
+      </c>
+      <c r="H21">
+        <v>23</v>
+      </c>
+      <c r="I21">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB76D1AB-0FA8-4084-A9B9-88592DF88B23}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>71</v>
+      </c>
+      <c r="D2">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>31</v>
+      </c>
+      <c r="F2">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>69</v>
+      </c>
+      <c r="D3">
+        <v>57</v>
+      </c>
+      <c r="E3">
+        <v>39</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>67</v>
+      </c>
+      <c r="D4">
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <v>35</v>
+      </c>
+      <c r="F4">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>67</v>
+      </c>
+      <c r="D5">
+        <v>60</v>
+      </c>
+      <c r="E5">
+        <v>38</v>
+      </c>
+      <c r="F5">
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>66</v>
+      </c>
+      <c r="D6">
+        <v>55</v>
+      </c>
+      <c r="E6">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>52</v>
+      </c>
+      <c r="E7">
+        <v>42</v>
+      </c>
+      <c r="F7">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>63</v>
+      </c>
+      <c r="D8">
+        <v>62</v>
+      </c>
+      <c r="E8">
+        <v>39</v>
+      </c>
+      <c r="F8">
+        <v>18</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>58</v>
+      </c>
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>32</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>58</v>
+      </c>
+      <c r="D10">
+        <v>58</v>
+      </c>
+      <c r="E10">
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <v>13</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>58</v>
+      </c>
+      <c r="E11">
+        <v>61</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>52</v>
+      </c>
+      <c r="D12">
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <v>36</v>
+      </c>
+      <c r="F12">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>13</v>
+      </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>49</v>
+      </c>
+      <c r="D13">
+        <v>48</v>
+      </c>
+      <c r="E13">
+        <v>43</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>49</v>
+      </c>
+      <c r="E14">
+        <v>54</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>46</v>
+      </c>
+      <c r="D15">
+        <v>31</v>
+      </c>
+      <c r="E15">
+        <v>49</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>16</v>
+      </c>
+      <c r="I15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>42</v>
+      </c>
+      <c r="D16">
+        <v>46</v>
+      </c>
+      <c r="E16">
+        <v>54</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="I16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>36</v>
+      </c>
+      <c r="E17">
+        <v>59</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>11</v>
+      </c>
+      <c r="H17">
+        <v>19</v>
+      </c>
+      <c r="I17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>38</v>
+      </c>
+      <c r="E18">
+        <v>59</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>22</v>
+      </c>
+      <c r="I18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>37</v>
+      </c>
+      <c r="E19">
+        <v>59</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>20</v>
+      </c>
+      <c r="I19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>26</v>
+      </c>
+      <c r="D20">
+        <v>41</v>
+      </c>
+      <c r="E20">
+        <v>61</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>14</v>
+      </c>
+      <c r="H20">
+        <v>20</v>
+      </c>
+      <c r="I20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>29</v>
+      </c>
+      <c r="E21">
+        <v>71</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <v>26</v>
+      </c>
+      <c r="I21">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED30DD2-EE9F-46F6-89BF-EAE4F6536EBA}">
   <dimension ref="A1:I21"/>
   <sheetViews>
@@ -3298,11 +5853,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55457669-E282-42E8-9ED5-53ED152F0351}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -3920,4 +6475,631 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5648DF-46E3-47A7-8B85-B724C232959F}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>82</v>
+      </c>
+      <c r="D2">
+        <v>78</v>
+      </c>
+      <c r="E2">
+        <v>38</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>76</v>
+      </c>
+      <c r="D3">
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>66</v>
+      </c>
+      <c r="D4">
+        <v>59</v>
+      </c>
+      <c r="E4">
+        <v>33</v>
+      </c>
+      <c r="F4">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>61</v>
+      </c>
+      <c r="D5">
+        <v>62</v>
+      </c>
+      <c r="E5">
+        <v>44</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>55</v>
+      </c>
+      <c r="D6">
+        <v>42</v>
+      </c>
+      <c r="E6">
+        <v>41</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
+      <c r="I6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <v>51</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>53</v>
+      </c>
+      <c r="D8">
+        <v>46</v>
+      </c>
+      <c r="E8">
+        <v>47</v>
+      </c>
+      <c r="F8">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>13</v>
+      </c>
+      <c r="I8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>52</v>
+      </c>
+      <c r="D9">
+        <v>52</v>
+      </c>
+      <c r="E9">
+        <v>43</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>14</v>
+      </c>
+      <c r="I9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>48</v>
+      </c>
+      <c r="D10">
+        <v>41</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>18</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>46</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>57</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
+      <c r="I11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>48</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="H12">
+        <v>13</v>
+      </c>
+      <c r="I12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <v>39</v>
+      </c>
+      <c r="E13">
+        <v>49</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>15</v>
+      </c>
+      <c r="I13">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>44</v>
+      </c>
+      <c r="D14">
+        <v>42</v>
+      </c>
+      <c r="E14">
+        <v>52</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <v>16</v>
+      </c>
+      <c r="I14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>44</v>
+      </c>
+      <c r="D15">
+        <v>47</v>
+      </c>
+      <c r="E15">
+        <v>56</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>14</v>
+      </c>
+      <c r="I15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>37</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>16</v>
+      </c>
+      <c r="H16">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>42</v>
+      </c>
+      <c r="D17">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>47</v>
+      </c>
+      <c r="F17">
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>18</v>
+      </c>
+      <c r="I17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>38</v>
+      </c>
+      <c r="E18">
+        <v>49</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>39</v>
+      </c>
+      <c r="D19">
+        <v>42</v>
+      </c>
+      <c r="E19">
+        <v>48</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+      <c r="G19">
+        <v>16</v>
+      </c>
+      <c r="H19">
+        <v>13</v>
+      </c>
+      <c r="I19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>39</v>
+      </c>
+      <c r="D20">
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>56</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <v>19</v>
+      </c>
+      <c r="I20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>32</v>
+      </c>
+      <c r="E21">
+        <v>56</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+      <c r="G21">
+        <v>13</v>
+      </c>
+      <c r="H21">
+        <v>18</v>
+      </c>
+      <c r="I21">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>